<commit_message>
Chair finished & implemented, barricade particles, standing_light fixed
</commit_message>
<xml_diff>
--- a/Art/Assets.xlsx
+++ b/Art/Assets.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7035E31C-9C45-4748-84F5-FFDC0399E6DB}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BF38A92-0AA9-4061-B5B5-C689177D0A90}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -494,8 +494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>